<commit_message>
agregue set de validacion
</commit_message>
<xml_diff>
--- a/ccd-incoloy.xlsx
+++ b/ccd-incoloy.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Cr ppm</t>
   </si>
@@ -420,7 +421,7 @@
         <v>290</v>
       </c>
       <c r="D2">
-        <v>0.075</v>
+        <v>0.1225</v>
       </c>
       <c r="E2">
         <v>0.05</v>
@@ -437,7 +438,7 @@
         <v>290</v>
       </c>
       <c r="D3">
-        <v>0.075</v>
+        <v>0.1225</v>
       </c>
       <c r="E3">
         <v>0.03</v>
@@ -454,7 +455,7 @@
         <v>290</v>
       </c>
       <c r="D4">
-        <v>0.075</v>
+        <v>0.1225</v>
       </c>
       <c r="E4">
         <v>0.03</v>
@@ -471,7 +472,7 @@
         <v>290</v>
       </c>
       <c r="D5">
-        <v>0.075</v>
+        <v>0.1225</v>
       </c>
       <c r="E5">
         <v>0.05</v>
@@ -488,7 +489,7 @@
         <v>430</v>
       </c>
       <c r="D6">
-        <v>0.075</v>
+        <v>0.1225</v>
       </c>
       <c r="E6">
         <v>0.03</v>
@@ -505,7 +506,7 @@
         <v>430</v>
       </c>
       <c r="D7">
-        <v>0.075</v>
+        <v>0.1225</v>
       </c>
       <c r="E7">
         <v>0.05</v>
@@ -522,7 +523,7 @@
         <v>430</v>
       </c>
       <c r="D8">
-        <v>0.075</v>
+        <v>0.1225</v>
       </c>
       <c r="E8">
         <v>0.05</v>
@@ -539,7 +540,7 @@
         <v>430</v>
       </c>
       <c r="D9">
-        <v>0.075</v>
+        <v>0.1225</v>
       </c>
       <c r="E9">
         <v>0.03</v>
@@ -556,7 +557,7 @@
         <v>290</v>
       </c>
       <c r="D10">
-        <v>0.125</v>
+        <v>0.2675</v>
       </c>
       <c r="E10">
         <v>0.03</v>
@@ -573,7 +574,7 @@
         <v>290</v>
       </c>
       <c r="D11">
-        <v>0.125</v>
+        <v>0.2675</v>
       </c>
       <c r="E11">
         <v>0.05</v>
@@ -590,7 +591,7 @@
         <v>290</v>
       </c>
       <c r="D12">
-        <v>0.125</v>
+        <v>0.2675</v>
       </c>
       <c r="E12">
         <v>0.05</v>
@@ -607,7 +608,7 @@
         <v>290</v>
       </c>
       <c r="D13">
-        <v>0.125</v>
+        <v>0.2675</v>
       </c>
       <c r="E13">
         <v>0.03</v>
@@ -624,7 +625,7 @@
         <v>430</v>
       </c>
       <c r="D14">
-        <v>0.125</v>
+        <v>0.2675</v>
       </c>
       <c r="E14">
         <v>0.05</v>
@@ -641,7 +642,7 @@
         <v>430</v>
       </c>
       <c r="D15">
-        <v>0.125</v>
+        <v>0.2675</v>
       </c>
       <c r="E15">
         <v>0.03</v>
@@ -658,7 +659,7 @@
         <v>430</v>
       </c>
       <c r="D16">
-        <v>0.125</v>
+        <v>0.2675</v>
       </c>
       <c r="E16">
         <v>0.03</v>
@@ -675,7 +676,7 @@
         <v>430</v>
       </c>
       <c r="D17">
-        <v>0.125</v>
+        <v>0.2675</v>
       </c>
       <c r="E17">
         <v>0.05</v>
@@ -692,7 +693,7 @@
         <v>360</v>
       </c>
       <c r="D18">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E18">
         <v>0.03999999999999999</v>
@@ -709,7 +710,7 @@
         <v>360</v>
       </c>
       <c r="D19">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E19">
         <v>0.03999999999999999</v>
@@ -726,7 +727,7 @@
         <v>500</v>
       </c>
       <c r="D20">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E20">
         <v>0.03999999999999999</v>
@@ -743,7 +744,7 @@
         <v>360</v>
       </c>
       <c r="D21">
-        <v>0.15</v>
+        <v>0.34</v>
       </c>
       <c r="E21">
         <v>0.03999999999999999</v>
@@ -760,7 +761,7 @@
         <v>360</v>
       </c>
       <c r="D22">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E22">
         <v>0.06</v>
@@ -777,7 +778,7 @@
         <v>360</v>
       </c>
       <c r="D23">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E23">
         <v>0.03999999999999999</v>
@@ -794,7 +795,7 @@
         <v>360</v>
       </c>
       <c r="D24">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E24">
         <v>0.03999999999999999</v>
@@ -811,7 +812,7 @@
         <v>220</v>
       </c>
       <c r="D25">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E25">
         <v>0.03999999999999999</v>
@@ -845,7 +846,7 @@
         <v>360</v>
       </c>
       <c r="D27">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E27">
         <v>0.02</v>
@@ -862,7 +863,7 @@
         <v>360</v>
       </c>
       <c r="D28">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E28">
         <v>0.03999999999999999</v>
@@ -879,7 +880,7 @@
         <v>360</v>
       </c>
       <c r="D29">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E29">
         <v>0.03999999999999999</v>
@@ -896,7 +897,7 @@
         <v>360</v>
       </c>
       <c r="D30">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E30">
         <v>0.03999999999999999</v>
@@ -913,7 +914,7 @@
         <v>360</v>
       </c>
       <c r="D31">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E31">
         <v>0.03999999999999999</v>
@@ -930,10 +931,176 @@
         <v>360</v>
       </c>
       <c r="D32">
-        <v>0.1</v>
+        <v>0.195</v>
       </c>
       <c r="E32">
         <v>0.03999999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>143.75</v>
+      </c>
+      <c r="B2">
+        <v>336.25</v>
+      </c>
+      <c r="C2">
+        <v>307.5</v>
+      </c>
+      <c r="D2">
+        <v>0.068125</v>
+      </c>
+      <c r="E2">
+        <v>0.05249999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>181.25</v>
+      </c>
+      <c r="B3">
+        <v>238.75</v>
+      </c>
+      <c r="C3">
+        <v>482.5</v>
+      </c>
+      <c r="D3">
+        <v>0.104375</v>
+      </c>
+      <c r="E3">
+        <v>0.0325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>193.75</v>
+      </c>
+      <c r="B4">
+        <v>303.75</v>
+      </c>
+      <c r="C4">
+        <v>342.5</v>
+      </c>
+      <c r="D4">
+        <v>0.249375</v>
+      </c>
+      <c r="E4">
+        <v>0.0375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>131.25</v>
+      </c>
+      <c r="B5">
+        <v>206.25</v>
+      </c>
+      <c r="C5">
+        <v>377.5</v>
+      </c>
+      <c r="D5">
+        <v>0.285625</v>
+      </c>
+      <c r="E5">
+        <v>0.0475</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>106.25</v>
+      </c>
+      <c r="B6">
+        <v>368.75</v>
+      </c>
+      <c r="C6">
+        <v>412.5</v>
+      </c>
+      <c r="D6">
+        <v>0.321875</v>
+      </c>
+      <c r="E6">
+        <v>0.0225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>156.25</v>
+      </c>
+      <c r="B7">
+        <v>433.75</v>
+      </c>
+      <c r="C7">
+        <v>447.5</v>
+      </c>
+      <c r="D7">
+        <v>0.213125</v>
+      </c>
+      <c r="E7">
+        <v>0.0575</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>168.75</v>
+      </c>
+      <c r="B8">
+        <v>401.25</v>
+      </c>
+      <c r="C8">
+        <v>272.5</v>
+      </c>
+      <c r="D8">
+        <v>0.176875</v>
+      </c>
+      <c r="E8">
+        <v>0.0275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>118.75</v>
+      </c>
+      <c r="B9">
+        <v>271.25</v>
+      </c>
+      <c r="C9">
+        <v>237.5</v>
+      </c>
+      <c r="D9">
+        <v>0.140625</v>
+      </c>
+      <c r="E9">
+        <v>0.0425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>